<commit_message>
add README.md, fix database
</commit_message>
<xml_diff>
--- a/excel/format-detail.xlsx
+++ b/excel/format-detail.xlsx
@@ -1,39 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp7\htdocs\waranti_daihatsu\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\waranti\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14A50173-CEDF-4673-AE53-815AC3B7DBD7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2835" yWindow="-11640" windowWidth="15600" windowHeight="11160" xr2:uid="{595068E8-D0B7-46BC-95E3-63005FB0C994}"/>
+    <workbookView minimized="1" xWindow="2835" yWindow="-11640" windowWidth="15600" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>NAMA KARYAWAN</t>
   </si>
@@ -66,12 +58,18 @@
   </si>
   <si>
     <t>VIN RANGKA</t>
+  </si>
+  <si>
+    <t>d78328s</t>
+  </si>
+  <si>
+    <t>bison</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -101,8 +99,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -416,11 +415,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95617D17-BAF0-4EB3-BF1B-9C5420BD077F}">
-  <dimension ref="A1:K1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -433,8 +432,8 @@
     <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.85546875" customWidth="1"/>
+    <col min="10" max="10" width="5.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -473,6 +472,35 @@
         <v>8</v>
       </c>
     </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C2">
+        <v>1110</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2">
+        <v>879</v>
+      </c>
+      <c r="F2" s="1">
+        <v>43628</v>
+      </c>
+      <c r="G2" s="1">
+        <v>43636</v>
+      </c>
+      <c r="H2">
+        <v>109230</v>
+      </c>
+      <c r="I2">
+        <v>888</v>
+      </c>
+      <c r="J2">
+        <v>8239</v>
+      </c>
+      <c r="K2" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>